<commit_message>
Ajustado modelo de banco de dados e Atualizado EsbocoDiagramaClasses.xlsx
Reinicio de Programação!!!
</commit_message>
<xml_diff>
--- a/Docs/ModelagemDataBase.xlsx
+++ b/Docs/ModelagemDataBase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="19875" windowHeight="7710"/>
+    <workbookView xWindow="-5595" yWindow="210" windowWidth="19875" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -759,6 +759,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="E11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+INT
+UNSIGNED
+NOT NULL</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G11" authorId="0">
       <text>
         <r>
@@ -891,32 +917,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-INT
-UNSIGNED
-NOT NULL</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="G13" authorId="0">
       <text>
         <r>
@@ -1016,8 +1016,8 @@
           </rPr>
           <t xml:space="preserve">
 INT
-NOT NULL
-UNSIGNED</t>
+UNSIGNED
+NOT NULL</t>
         </r>
       </text>
     </comment>
@@ -1047,6 +1047,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="E15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+INT
+NOT NULL
+UNSIGNED</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G16" authorId="0">
       <text>
         <r>
@@ -1101,7 +1127,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="0">
+    <comment ref="G17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+TINYINT
+NOT NULL
+UNSIGNED</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1128,7 +1180,367 @@
         </r>
       </text>
     </comment>
-    <comment ref="G17" authorId="0">
+    <comment ref="C18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+VARCHAR(20)
+NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+INT
+UNSIGNED
+NOT NULL
+AUTO_INCREMENT</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+CHAR(1)
+NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+INT
+UNSIGNED
+NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+INT
+UNSIGNED
+NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+INT
+UNSIGNED
+NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+INT
+UNSIGNED
+NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+INT
+NOT NULL
+UNSIGNED</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+INT
+NOT NULL
+UNSIGNED</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+INT
+UNSIGNED
+NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+TINYINT
+UNSIGNED
+NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+TINYINT
+NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+INT
+UNSIGNED
+NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Igor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FLOAT</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1151,392 +1563,6 @@
 TINYINT
 NOT NULL
 UNSIGNED</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A18" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-INT
-UNSIGNED
-NOT NULL
-AUTO_INCREMENT</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C18" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-VARCHAR(20)
-NOT NULL</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E18" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-INT
-UNSIGNED
-NOT NULL</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G18" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-CHAR(1)
-NOT NULL</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A19" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-INT
-UNSIGNED
-NOT NULL</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C19" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-INT
-UNSIGNED
-NOT NULL</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E19" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-INT
-NOT NULL
-UNSIGNED</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G19" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-INT
-UNSIGNED
-NOT NULL</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A20" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-INT
-NOT NULL
-UNSIGNED</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E20" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-TINYINT
-NOT NULL</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G20" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-INT
-UNSIGNED
-NOT NULL</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A21" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-TINYINT
-UNSIGNED
-NOT NULL</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E21" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-TINYINT
-NOT NULL
-UNSIGNED</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G21" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-INT
-UNSIGNED
-NOT NULL</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A22" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Igor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-FLOAT</t>
         </r>
       </text>
     </comment>
@@ -1647,7 +1673,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
   <si>
     <t>ID</t>
   </si>
@@ -1836,6 +1862,9 @@
   </si>
   <si>
     <t>CHAVE PRIMARIA</t>
+  </si>
+  <si>
+    <t>TURMA = TURMA(ID)</t>
   </si>
 </sst>
 </file>
@@ -2265,8 +2294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2408,7 +2437,7 @@
       <c r="A10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -2419,6 +2448,9 @@
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="E11" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="G11" s="6" t="s">
         <v>0</v>
       </c>
@@ -2430,9 +2462,6 @@
       <c r="C12" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="G12" s="8" t="s">
         <v>43</v>
       </c>
@@ -2444,8 +2473,8 @@
       <c r="C13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>46</v>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>44</v>
@@ -2458,14 +2487,17 @@
       <c r="C14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>47</v>
+      <c r="E14" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
         <v>44</v>
       </c>
+      <c r="E15" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>37</v>
       </c>
@@ -2474,9 +2506,6 @@
       <c r="C16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="G16" s="6" t="s">
         <v>0</v>
       </c>
@@ -2488,8 +2517,8 @@
       <c r="C17" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>0</v>
+      <c r="E17" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>26</v>
@@ -2502,8 +2531,8 @@
       <c r="C18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>55</v>
+      <c r="E18" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>27</v>
@@ -2517,7 +2546,7 @@
         <v>45</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>48</v>
@@ -2528,7 +2557,7 @@
         <v>47</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>49</v>
@@ -2538,8 +2567,8 @@
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>31</v>
+      <c r="E21" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>50</v>
@@ -2550,6 +2579,9 @@
         <v>30</v>
       </c>
       <c r="C22" s="12"/>
+      <c r="E22" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="G22" s="4" t="s">
         <v>51</v>
       </c>

</xml_diff>